<commit_message>
added feature to conceal dates not designated as 'public' when publishing to frontend
</commit_message>
<xml_diff>
--- a/import_sample.xlsx
+++ b/import_sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\documents_synced\Arch14CZ\arch14cz_backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3688D15-AA1F-498B-A711-271E41EB5977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC30676-E65F-49E7-9812-069B72401674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{A98429E4-2D3D-4224-A534-358619287A32}"/>
+    <workbookView xWindow="3456" yWindow="3456" windowWidth="23040" windowHeight="12204" xr2:uid="{A98429E4-2D3D-4224-A534-358619287A32}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="98">
   <si>
     <t>14C Analysis_Lab code</t>
   </si>
@@ -326,6 +326,9 @@
   </si>
   <si>
     <t>Moravian Painted Ware, phase Ia</t>
+  </si>
+  <si>
+    <t>Public</t>
   </si>
 </sst>
 </file>
@@ -400,67 +403,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -831,46 +774,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9340F97-C2A2-4016-9BA8-8EE7FC7B8D19}">
-  <dimension ref="A1:AG5"/>
+  <dimension ref="A1:AH5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="20" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="30.6640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="16" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="29" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="53.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="30" width="22.28515625" customWidth="1"/>
+    <col min="25" max="25" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="53.5546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="30" width="22.33203125" customWidth="1"/>
     <col min="31" max="31" width="18" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="6.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -970,8 +914,11 @@
       <c r="AG1" s="1" t="s">
         <v>81</v>
       </c>
+      <c r="AH1" s="1" t="s">
+        <v>97</v>
+      </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>38</v>
       </c>
@@ -1065,8 +1012,11 @@
       <c r="AG2" t="s">
         <v>82</v>
       </c>
+      <c r="AH2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>54</v>
       </c>
@@ -1163,8 +1113,11 @@
       <c r="AG3" t="s">
         <v>82</v>
       </c>
+      <c r="AH3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>65</v>
       </c>
@@ -1258,8 +1211,11 @@
       <c r="AG4" t="s">
         <v>82</v>
       </c>
+      <c r="AH4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>85</v>
       </c>
@@ -1340,20 +1296,23 @@
       </c>
       <c r="AG5" t="s">
         <v>82</v>
+      </c>
+      <c r="AH5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="11" priority="11"/>
-    <cfRule type="duplicateValues" dxfId="10" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A4">
-    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="4" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
removed Dating_Type field; unpublished dates no longer exported to frontend;
</commit_message>
<xml_diff>
--- a/import_sample.xlsx
+++ b/import_sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\documents_synced\Arch14CZ\arch14cz_backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC30676-E65F-49E7-9812-069B72401674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CAC06D4-618A-421D-B2DC-577562709272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3456" yWindow="3456" windowWidth="23040" windowHeight="12204" xr2:uid="{A98429E4-2D3D-4224-A534-358619287A32}"/>
+    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8964" xr2:uid="{A98429E4-2D3D-4224-A534-358619287A32}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="96">
   <si>
     <t>14C Analysis_Lab code</t>
   </si>
@@ -46,9 +46,6 @@
     <t>14C Analysis_14C uncert. 1 sig</t>
   </si>
   <si>
-    <t>Date_type</t>
-  </si>
-  <si>
     <t>14C Analysis_14C Method</t>
   </si>
   <si>
@@ -130,9 +127,6 @@
     <t>Source_acquisition</t>
   </si>
   <si>
-    <t>conv. 14C BP</t>
-  </si>
-  <si>
     <t>conventional</t>
   </si>
   <si>
@@ -148,9 +142,6 @@
     <t>AMS</t>
   </si>
   <si>
-    <t>animal bone</t>
-  </si>
-  <si>
     <t>Poz-102430</t>
   </si>
   <si>
@@ -184,9 +175,6 @@
     <t>Linear Pottery Culture</t>
   </si>
   <si>
-    <t>charred botanical macroremain</t>
-  </si>
-  <si>
     <t>in contradiction with archaeological chronology/sequence</t>
   </si>
   <si>
@@ -226,9 +214,6 @@
     <t>18..2003</t>
   </si>
   <si>
-    <t>charred grain</t>
-  </si>
-  <si>
     <t>Panicum miliaceum</t>
   </si>
   <si>
@@ -329,6 +314,15 @@
   </si>
   <si>
     <t>Public</t>
+  </si>
+  <si>
+    <t>bone, animal</t>
+  </si>
+  <si>
+    <t>grain, charred</t>
+  </si>
+  <si>
+    <t>botanical macroremain, charred</t>
   </si>
 </sst>
 </file>
@@ -774,47 +768,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9340F97-C2A2-4016-9BA8-8EE7FC7B8D19}">
-  <dimension ref="A1:AH5"/>
+  <dimension ref="A1:AG5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="29" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="53.5546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="30" width="22.33203125" customWidth="1"/>
-    <col min="31" max="31" width="18" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="29" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="53.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="22.33203125" customWidth="1"/>
+    <col min="30" max="30" width="18" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -860,16 +855,16 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="T1" s="1" t="s">
@@ -906,21 +901,18 @@
         <v>29</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B2">
         <v>1295</v>
@@ -928,97 +920,94 @@
       <c r="C2">
         <v>30</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2">
+        <v>0.3</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="H2" t="s">
         <v>36</v>
       </c>
-      <c r="F2">
-        <v>0.3</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2">
+        <v>742503</v>
+      </c>
+      <c r="J2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>43</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="U2" s="3">
+        <v>2690</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="W2" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD2" t="s">
         <v>33</v>
       </c>
-      <c r="I2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2">
-        <v>742503</v>
-      </c>
-      <c r="K2" t="s">
-        <v>40</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="M2" t="s">
-        <v>42</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="P2" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="R2" t="s">
-        <v>46</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="V2" s="3">
-        <v>2690</v>
-      </c>
-      <c r="W2" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="X2" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z2" t="s">
+      <c r="AE2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC2" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="B3">
         <v>3065</v>
@@ -1026,100 +1015,97 @@
       <c r="C3">
         <v>35</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3">
+        <v>-17.2</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3">
-        <v>-17.2</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>84</v>
-      </c>
       <c r="H3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3">
+        <v>720755</v>
+      </c>
+      <c r="J3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3" t="s">
+        <v>53</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="X3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD3" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J3">
-        <v>720755</v>
-      </c>
-      <c r="K3" t="s">
-        <v>55</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="M3" t="s">
-        <v>57</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="S3" s="5" t="s">
+      <c r="AE3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>60</v>
-      </c>
-      <c r="T3" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="V3" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="W3" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="X3" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>64</v>
-      </c>
-      <c r="Z3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>79</v>
-      </c>
-      <c r="AB3" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC3" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>83</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>65</v>
       </c>
       <c r="B4">
         <v>5840</v>
@@ -1128,96 +1114,93 @@
         <v>30</v>
       </c>
       <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4">
+        <v>-20.3</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G4" t="s">
         <v>31</v>
       </c>
-      <c r="E4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4">
-        <v>-20.3</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>84</v>
-      </c>
       <c r="H4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I4">
+        <v>668150</v>
+      </c>
+      <c r="J4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K4" t="s">
+        <v>62</v>
+      </c>
+      <c r="L4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="N4" t="s">
+        <v>64</v>
+      </c>
+      <c r="O4" t="s">
+        <v>65</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>67</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="S4" t="s">
+        <v>69</v>
+      </c>
+      <c r="U4" t="s">
+        <v>70</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="W4" t="s">
+        <v>93</v>
+      </c>
+      <c r="Y4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD4" t="s">
         <v>33</v>
       </c>
-      <c r="I4" t="s">
-        <v>66</v>
-      </c>
-      <c r="J4">
-        <v>668150</v>
-      </c>
-      <c r="K4" t="s">
-        <v>66</v>
-      </c>
-      <c r="L4" t="s">
-        <v>67</v>
-      </c>
-      <c r="M4" t="s">
-        <v>68</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="O4" t="s">
-        <v>69</v>
-      </c>
-      <c r="P4" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="R4" t="s">
-        <v>72</v>
-      </c>
-      <c r="S4" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="T4" t="s">
-        <v>74</v>
-      </c>
-      <c r="V4" t="s">
-        <v>75</v>
-      </c>
-      <c r="W4" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="X4" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>79</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>76</v>
-      </c>
-      <c r="AC4" t="s">
+      <c r="AE4" t="s">
+        <v>78</v>
+      </c>
+      <c r="AF4" t="s">
         <v>77</v>
       </c>
-      <c r="AD4" t="s">
-        <v>78</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>35</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>83</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH4">
+      <c r="AG4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B5">
         <v>4955</v>
@@ -1226,78 +1209,75 @@
         <v>80</v>
       </c>
       <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5" t="s">
         <v>31</v>
       </c>
-      <c r="E5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" t="s">
+        <v>81</v>
+      </c>
+      <c r="I5">
+        <v>678554</v>
+      </c>
+      <c r="J5" t="s">
+        <v>82</v>
+      </c>
+      <c r="K5" t="s">
+        <v>83</v>
+      </c>
+      <c r="L5" t="s">
         <v>84</v>
       </c>
-      <c r="H5" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="N5" t="s">
+        <v>64</v>
+      </c>
+      <c r="O5" t="s">
+        <v>65</v>
+      </c>
+      <c r="P5" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="S5" t="s">
+        <v>90</v>
+      </c>
+      <c r="T5" t="s">
+        <v>91</v>
+      </c>
+      <c r="U5" t="s">
+        <v>89</v>
+      </c>
+      <c r="V5" t="s">
+        <v>89</v>
+      </c>
+      <c r="W5" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA5" t="s">
         <v>86</v>
       </c>
-      <c r="J5">
-        <v>678554</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="AC5" t="s">
         <v>87</v>
       </c>
-      <c r="L5" t="s">
+      <c r="AD5" t="s">
         <v>88</v>
       </c>
-      <c r="M5" t="s">
-        <v>89</v>
-      </c>
-      <c r="O5" t="s">
-        <v>69</v>
-      </c>
-      <c r="P5" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>94</v>
-      </c>
-      <c r="R5" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="T5" t="s">
-        <v>95</v>
-      </c>
-      <c r="U5" t="s">
-        <v>96</v>
-      </c>
-      <c r="V5" t="s">
-        <v>94</v>
-      </c>
-      <c r="W5" t="s">
-        <v>94</v>
-      </c>
-      <c r="X5" t="s">
-        <v>90</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>91</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>92</v>
-      </c>
       <c r="AE5" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="AF5" t="s">
-        <v>83</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH5">
+        <v>77</v>
+      </c>
+      <c r="AG5">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added separate commands to order relative dates, calibrate dates and generate Arch14CZ IDs; added possibility to export records without a C-14 date or 1sigma to the frontend;
</commit_message>
<xml_diff>
--- a/import_sample.xlsx
+++ b/import_sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\documents_synced\Arch14CZ\arch14cz_backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93464114-1B97-442D-B12F-1C02E529B61F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E488C9-0E1A-4BEE-9D04-D9076E8CE0E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1908" yWindow="3732" windowWidth="23040" windowHeight="12204" xr2:uid="{A98429E4-2D3D-4224-A534-358619287A32}"/>
+    <workbookView xWindow="4872" yWindow="4152" windowWidth="23040" windowHeight="12204" xr2:uid="{A98429E4-2D3D-4224-A534-358619287A32}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,25 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="101">
-  <si>
-    <t>14C Analysis_Lab code</t>
-  </si>
-  <si>
-    <t>14C Analysis_14C activity BP</t>
-  </si>
-  <si>
-    <t>14C Analysis_14C uncert. 1 sig</t>
-  </si>
-  <si>
-    <t>14C Analysis_14C Method</t>
-  </si>
-  <si>
-    <t>Delta_13C</t>
-  </si>
-  <si>
-    <t>14C Analysis.Note</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="100">
   <si>
     <t>Country</t>
   </si>
@@ -61,72 +43,15 @@
     <t>Cadastre</t>
   </si>
   <si>
-    <t>Cadastre_Code</t>
-  </si>
-  <si>
     <t>District</t>
   </si>
   <si>
-    <t>Site_Name</t>
-  </si>
-  <si>
-    <t>Site_Coordinates</t>
-  </si>
-  <si>
-    <t>Site_Note</t>
-  </si>
-  <si>
-    <t>Activity_Area</t>
-  </si>
-  <si>
     <t>Feature</t>
   </si>
   <si>
-    <t>Context_Name</t>
-  </si>
-  <si>
-    <t>Context_Description</t>
-  </si>
-  <si>
-    <t>Depth_cm</t>
-  </si>
-  <si>
-    <t>Relative dating_Name1</t>
-  </si>
-  <si>
-    <t>Relative dating_Name2</t>
-  </si>
-  <si>
-    <t>Sample_Number</t>
-  </si>
-  <si>
-    <t>Sample_Note</t>
-  </si>
-  <si>
-    <t>Material_Name</t>
-  </si>
-  <si>
-    <t>Material_Note</t>
-  </si>
-  <si>
     <t>Reliability</t>
   </si>
   <si>
-    <t>Reliability_Note</t>
-  </si>
-  <si>
-    <t>Source_Description</t>
-  </si>
-  <si>
-    <t>Source_Reference</t>
-  </si>
-  <si>
-    <t>Source_URI</t>
-  </si>
-  <si>
-    <t>Source_acquisition</t>
-  </si>
-  <si>
     <t>conventional</t>
   </si>
   <si>
@@ -262,12 +187,6 @@
     <t>Reliability Note</t>
   </si>
   <si>
-    <t>Submitter_Name</t>
-  </si>
-  <si>
-    <t>Submitter_Organization</t>
-  </si>
-  <si>
     <t>Organization</t>
   </si>
   <si>
@@ -325,9 +244,6 @@
     <t>botanical macroremain, charred</t>
   </si>
   <si>
-    <t>AMCR_ID</t>
-  </si>
-  <si>
     <t>C-9124798A</t>
   </si>
   <si>
@@ -338,6 +254,87 @@
   </si>
   <si>
     <t>C-9156591A</t>
+  </si>
+  <si>
+    <t>Lab Code</t>
+  </si>
+  <si>
+    <t>C-14 Activity BP</t>
+  </si>
+  <si>
+    <t>C-14 Uncert. 1 Sigma</t>
+  </si>
+  <si>
+    <t>C-14 Method</t>
+  </si>
+  <si>
+    <t>Delta C-13</t>
+  </si>
+  <si>
+    <t>C-14 Analysis Note</t>
+  </si>
+  <si>
+    <t>Cadastre Code</t>
+  </si>
+  <si>
+    <t>Site Name</t>
+  </si>
+  <si>
+    <t>Site Coordinates</t>
+  </si>
+  <si>
+    <t>Site Note</t>
+  </si>
+  <si>
+    <t>AMCR ID</t>
+  </si>
+  <si>
+    <t>Activity Area</t>
+  </si>
+  <si>
+    <t>Context Name</t>
+  </si>
+  <si>
+    <t>Context Description</t>
+  </si>
+  <si>
+    <t>Depth cm</t>
+  </si>
+  <si>
+    <t>Relative Dating Name 1</t>
+  </si>
+  <si>
+    <t>Relative Dating Name 2</t>
+  </si>
+  <si>
+    <t>Sample Number</t>
+  </si>
+  <si>
+    <t>Sample Note</t>
+  </si>
+  <si>
+    <t>Material Name</t>
+  </si>
+  <si>
+    <t>Material Note</t>
+  </si>
+  <si>
+    <t>Source Description</t>
+  </si>
+  <si>
+    <t>Source Reference</t>
+  </si>
+  <si>
+    <t>Source URI</t>
+  </si>
+  <si>
+    <t>Source Acquisition</t>
+  </si>
+  <si>
+    <t>Submitter Name</t>
+  </si>
+  <si>
+    <t>Submitter Organization</t>
   </si>
 </sst>
 </file>
@@ -794,39 +791,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9340F97-C2A2-4016-9BA8-8EE7FC7B8D19}">
   <dimension ref="A1:AH5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="29" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="53.5546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="49.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="28" max="30" width="22.33203125" customWidth="1"/>
     <col min="31" max="31" width="18" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="16.33203125" bestFit="1" customWidth="1"/>
@@ -836,111 +831,111 @@
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="AE1" s="1" t="s">
-        <v>29</v>
+        <v>97</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>92</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>1295</v>
@@ -949,88 +944,88 @@
         <v>30</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="E2">
         <v>0.3</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="H2" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="I2">
         <v>742503</v>
       </c>
       <c r="J2" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="L2" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="P2" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="R2" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="V2" s="3">
         <v>2690</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="X2" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="Z2" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="AA2" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="AB2" s="4" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="AC2" s="4" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="AD2" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="AE2" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="AF2" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="AG2" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="AH2">
         <v>1</v>
@@ -1038,7 +1033,7 @@
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="B3">
         <v>3065</v>
@@ -1047,91 +1042,91 @@
         <v>35</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="E3">
         <v>-17.2</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="I3">
         <v>720755</v>
       </c>
       <c r="J3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="X3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF3" t="s">
         <v>51</v>
       </c>
-      <c r="K3" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="L3" t="s">
-        <v>53</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="S3" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="T3" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="V3" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="W3" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="X3" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AB3" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="AC3" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>78</v>
-      </c>
       <c r="AG3" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="AH3">
         <v>1</v>
@@ -1139,7 +1134,7 @@
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="B4">
         <v>5840</v>
@@ -1148,88 +1143,88 @@
         <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="E4">
         <v>-20.3</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="H4" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="I4">
         <v>668150</v>
       </c>
       <c r="J4" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="K4" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="L4" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
       <c r="O4" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="P4" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="Q4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="R4" t="s">
+        <v>42</v>
+      </c>
+      <c r="S4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="T4" t="s">
+        <v>44</v>
+      </c>
+      <c r="V4" t="s">
+        <v>45</v>
+      </c>
+      <c r="W4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="X4" t="s">
         <v>66</v>
       </c>
-      <c r="R4" t="s">
-        <v>67</v>
-      </c>
-      <c r="S4" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="T4" t="s">
-        <v>69</v>
-      </c>
-      <c r="V4" t="s">
-        <v>70</v>
-      </c>
-      <c r="W4" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="X4" t="s">
-        <v>93</v>
-      </c>
       <c r="Z4" s="4" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="AA4" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="AB4" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="AC4" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="AD4" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="AE4" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="AF4" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="AG4" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="AH4">
         <v>1</v>
@@ -1237,7 +1232,7 @@
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="B5">
         <v>4955</v>
@@ -1246,76 +1241,79 @@
         <v>80</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="G5" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="H5" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="I5">
         <v>678554</v>
       </c>
       <c r="J5" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="K5" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="L5" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="O5" t="s">
+        <v>39</v>
+      </c>
+      <c r="P5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="T5" t="s">
+        <v>63</v>
+      </c>
+      <c r="U5" t="s">
         <v>64</v>
       </c>
-      <c r="P5" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>89</v>
-      </c>
-      <c r="R5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="T5" t="s">
-        <v>90</v>
-      </c>
-      <c r="U5" t="s">
-        <v>91</v>
-      </c>
       <c r="V5" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="W5" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="X5" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="Z5" t="s">
-        <v>46</v>
+        <v>21</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>49</v>
       </c>
       <c r="AB5" t="s">
-        <v>86</v>
+        <v>59</v>
       </c>
       <c r="AD5" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="AE5" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="AF5" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="AG5" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="AH5">
         <v>0</v>

</xml_diff>

<commit_message>
added validation of some dictionary fields when importing
</commit_message>
<xml_diff>
--- a/import_sample.xlsx
+++ b/import_sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\documents_synced\Arch14CZ\arch14cz_backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E37CAB8-0335-4BDD-87F9-D991D1607B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F01ECA7-0FF4-4736-853A-1B437B07B3EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{A98429E4-2D3D-4224-A534-358619287A32}"/>
   </bookViews>
@@ -2678,27 +2678,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3091,7 +3071,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9340F97-C2A2-4016-9BA8-8EE7FC7B8D19}">
   <dimension ref="A1:AH171"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -17823,16 +17805,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="9" priority="11"/>
-    <cfRule type="duplicateValues" dxfId="8" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A4">
-    <cfRule type="duplicateValues" dxfId="7" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>